<commit_message>
updated ZIP Code to ZIP_code
</commit_message>
<xml_diff>
--- a/Data/Detroit Rates.xlsx
+++ b/Data/Detroit Rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmymiller/Library/Mobile Documents/com~apple~CloudDocs/Stat 300/STAT-300-Fa20/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C62EA54D-4467-C04F-9851-5D339799DC28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A399A6-B846-9B46-AE17-04F143257272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11280" yWindow="1660" windowWidth="17260" windowHeight="14440" xr2:uid="{97C615E2-605A-AE44-B0FB-D0C0A75923DB}"/>
   </bookViews>
@@ -35,13 +35,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>ZIP Code</t>
-  </si>
-  <si>
     <t>Deaths_per_HundThou</t>
   </si>
   <si>
     <t>Cases_per_HundThou</t>
+  </si>
+  <si>
+    <t>ZIP_Code</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A2:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -407,13 +407,13 @@
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>